<commit_message>
Pavel - new user for linking test
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C766679
</commit_message>
<xml_diff>
--- a/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="147">
   <si>
     <t>UserName</t>
   </si>
@@ -448,14 +448,22 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Linking_AutoUser</t>
+  </si>
+  <si>
+    <t>Default user for Linking tests</t>
+  </si>
+  <si>
+    <t>linking.autouser@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,7 +614,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -641,7 +649,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -850,18 +858,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1875,6 +1885,25 @@
       </c>
       <c r="G51" s="6" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1916,18 +1945,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
Usman - New users added to cobaltUsers.xls
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C771130
</commit_message>
<xml_diff>
--- a/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="274">
   <si>
     <t>UserName</t>
   </si>
@@ -640,13 +640,211 @@
   </si>
   <si>
     <t>tr-anz-tester2@yandex.com</t>
+  </si>
+  <si>
+    <t>KHPaddUser1</t>
+  </si>
+  <si>
+    <t>KHPaddUser2</t>
+  </si>
+  <si>
+    <t>KHPaddUser3</t>
+  </si>
+  <si>
+    <t>KHPaddUser4</t>
+  </si>
+  <si>
+    <t>KHPaddUser5</t>
+  </si>
+  <si>
+    <t>KHPaddUser6</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser1</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser2</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser3</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser4</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser5</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser6</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser7</t>
+  </si>
+  <si>
+    <t>SearchWhatsMarketUser8</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser1</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser2</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser3</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser4</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser5</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser6</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser7</t>
+  </si>
+  <si>
+    <t>SearchKnowHowUser8</t>
+  </si>
+  <si>
+    <t>AskUser1</t>
+  </si>
+  <si>
+    <t>AskUser2</t>
+  </si>
+  <si>
+    <t>AskUser3</t>
+  </si>
+  <si>
+    <t>AskUser4</t>
+  </si>
+  <si>
+    <t>AskUser5</t>
+  </si>
+  <si>
+    <t>AskUser6</t>
+  </si>
+  <si>
+    <t>AssetPageUser1</t>
+  </si>
+  <si>
+    <t>AssetPageUser2</t>
+  </si>
+  <si>
+    <t>AssetPageUser3</t>
+  </si>
+  <si>
+    <t>AssetPageUser4</t>
+  </si>
+  <si>
+    <t>AssetPageUser5</t>
+  </si>
+  <si>
+    <t>KHPaddUser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>KHPaddUser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>KHPaddUser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>KHPaddUser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>KHPaddUser5@mailinator.com</t>
+  </si>
+  <si>
+    <t>KHPaddUser6@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser2@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser3@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser4@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser6@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser7@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchWhatsMarketUser8@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser2@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser3@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser4@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser6@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser7@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchKnowHowUser8@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AskUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AskUser2@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AskUser3@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AskUser4@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AskUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AskUser6@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssetPageUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssetPageUser2@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssetPageUser3@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssetPageUser4@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssetPageUser5@mailinator.com </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,6 +867,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -737,7 +940,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -749,6 +952,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1054,15 +1258,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
@@ -2576,6 +2780,567 @@
       </c>
       <c r="G80" s="10" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B81" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B83" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B84" t="s">
+        <v>52</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B87" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B88" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B92" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B93" t="s">
+        <v>52</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B94" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B96" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="B97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B98" t="s">
+        <v>52</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B99" t="s">
+        <v>52</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B100" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B101" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B102" t="s">
+        <v>52</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G102" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G103" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B104" t="s">
+        <v>52</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B105" t="s">
+        <v>52</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G105" s="10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B106" t="s">
+        <v>52</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G108" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B109" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G109" s="10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B111" t="s">
+        <v>52</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2625,9 +3390,40 @@
     <hyperlink ref="G78" r:id="rId43"/>
     <hyperlink ref="G79" r:id="rId44"/>
     <hyperlink ref="G80" r:id="rId45"/>
+    <hyperlink ref="G82" r:id="rId46"/>
+    <hyperlink ref="G83" r:id="rId47"/>
+    <hyperlink ref="G84" r:id="rId48"/>
+    <hyperlink ref="G85" r:id="rId49"/>
+    <hyperlink ref="G86" r:id="rId50"/>
+    <hyperlink ref="G87" r:id="rId51"/>
+    <hyperlink ref="G88" r:id="rId52"/>
+    <hyperlink ref="G89" r:id="rId53"/>
+    <hyperlink ref="G90" r:id="rId54"/>
+    <hyperlink ref="G91" r:id="rId55"/>
+    <hyperlink ref="G92" r:id="rId56"/>
+    <hyperlink ref="G93" r:id="rId57"/>
+    <hyperlink ref="G94" r:id="rId58"/>
+    <hyperlink ref="G95" r:id="rId59"/>
+    <hyperlink ref="G96" r:id="rId60"/>
+    <hyperlink ref="G97" r:id="rId61"/>
+    <hyperlink ref="G98" r:id="rId62"/>
+    <hyperlink ref="G99" r:id="rId63"/>
+    <hyperlink ref="G100" r:id="rId64"/>
+    <hyperlink ref="G101" r:id="rId65"/>
+    <hyperlink ref="G102" r:id="rId66"/>
+    <hyperlink ref="G103" r:id="rId67"/>
+    <hyperlink ref="G104" r:id="rId68"/>
+    <hyperlink ref="G105" r:id="rId69"/>
+    <hyperlink ref="G106" r:id="rId70"/>
+    <hyperlink ref="G107" r:id="rId71"/>
+    <hyperlink ref="G108" r:id="rId72"/>
+    <hyperlink ref="G109" r:id="rId73"/>
+    <hyperlink ref="G110" r:id="rId74"/>
+    <hyperlink ref="G113" r:id="rId75"/>
+    <hyperlink ref="G111" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Oleg Babak - Production default user Oleg_Babak was added to CobaltUsers.xlsx's
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C778955
</commit_message>
<xml_diff>
--- a/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="276">
   <si>
     <t>UserName</t>
   </si>
@@ -838,6 +838,12 @@
   </si>
   <si>
     <t xml:space="preserve">AssetPageUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t>Oleg_Babak</t>
+  </si>
+  <si>
+    <t>Password1!</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1020,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1049,7 +1055,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1258,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,10 +1876,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>75</v>
+        <v>274</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>52</v>
+        <v>275</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
@@ -1889,26 +1895,26 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E32" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>82</v>
@@ -1916,134 +1922,130 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="F34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>93</v>
+      <c r="G34" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="D35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="F36" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>98</v>
+      <c r="G38" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>102</v>
+      <c r="G39" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>52</v>
@@ -2055,70 +2057,72 @@
         <v>33</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E41" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>110</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="5"/>
+      <c r="G42" s="6" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>25</v>
@@ -2127,49 +2131,51 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="5" t="s">
+      <c r="F45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>52</v>
@@ -2183,94 +2189,94 @@
         <v>25</v>
       </c>
       <c r="G46" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="8" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="E50" s="5" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>52</v>
@@ -2284,12 +2290,12 @@
         <v>25</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>52</v>
@@ -2297,35 +2303,37 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="5" t="s">
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>147</v>
-      </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
@@ -2337,12 +2345,12 @@
         <v>25</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
@@ -2354,12 +2362,12 @@
         <v>25</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
@@ -2371,12 +2379,12 @@
         <v>25</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
@@ -2388,12 +2396,12 @@
         <v>25</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
         <v>52</v>
@@ -2405,12 +2413,12 @@
         <v>25</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
@@ -2422,12 +2430,12 @@
         <v>25</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
@@ -2439,12 +2447,12 @@
         <v>25</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
@@ -2456,12 +2464,12 @@
         <v>25</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
@@ -2473,12 +2481,12 @@
         <v>25</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
@@ -2490,12 +2498,12 @@
         <v>25</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
@@ -2507,12 +2515,12 @@
         <v>25</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
@@ -2524,12 +2532,12 @@
         <v>25</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
@@ -2541,12 +2549,12 @@
         <v>25</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2558,12 +2566,12 @@
         <v>25</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B68" t="s">
         <v>52</v>
@@ -2575,12 +2583,12 @@
         <v>25</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
@@ -2592,12 +2600,12 @@
         <v>25</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
@@ -2609,12 +2617,12 @@
         <v>25</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B71" t="s">
         <v>52</v>
@@ -2626,12 +2634,12 @@
         <v>25</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
@@ -2643,12 +2651,12 @@
         <v>25</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
@@ -2660,12 +2668,12 @@
         <v>25</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
@@ -2677,12 +2685,12 @@
         <v>25</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
         <v>52</v>
@@ -2694,12 +2702,12 @@
         <v>25</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B76" t="s">
         <v>52</v>
@@ -2711,12 +2719,12 @@
         <v>25</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
@@ -2728,12 +2736,12 @@
         <v>25</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
         <v>52</v>
@@ -2745,12 +2753,12 @@
         <v>25</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B79" t="s">
         <v>52</v>
@@ -2762,46 +2770,46 @@
         <v>25</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>173</v>
+      </c>
+      <c r="B80" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>174</v>
       </c>
-      <c r="B80" t="s">
-        <v>52</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G80" s="10" t="s">
+      <c r="B81" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="10" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B81" t="s">
-        <v>52</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G81" s="10" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B82" t="s">
         <v>52</v>
@@ -2813,12 +2821,12 @@
         <v>25</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B83" t="s">
         <v>52</v>
@@ -2830,12 +2838,12 @@
         <v>25</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B84" t="s">
         <v>52</v>
@@ -2847,12 +2855,12 @@
         <v>25</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B85" t="s">
         <v>52</v>
@@ -2864,12 +2872,12 @@
         <v>25</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B86" t="s">
         <v>52</v>
@@ -2881,12 +2889,12 @@
         <v>25</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B87" t="s">
         <v>52</v>
@@ -2898,12 +2906,12 @@
         <v>25</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B88" t="s">
         <v>52</v>
@@ -2915,12 +2923,12 @@
         <v>25</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
@@ -2932,12 +2940,12 @@
         <v>25</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
@@ -2949,12 +2957,12 @@
         <v>25</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B91" t="s">
         <v>52</v>
@@ -2966,12 +2974,12 @@
         <v>25</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B92" t="s">
         <v>52</v>
@@ -2983,12 +2991,12 @@
         <v>25</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B93" t="s">
         <v>52</v>
@@ -3000,12 +3008,12 @@
         <v>25</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B94" t="s">
         <v>52</v>
@@ -3017,12 +3025,12 @@
         <v>25</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B95" t="s">
         <v>52</v>
@@ -3034,12 +3042,12 @@
         <v>25</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B96" t="s">
         <v>52</v>
@@ -3051,12 +3059,12 @@
         <v>25</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B97" t="s">
         <v>52</v>
@@ -3068,12 +3076,12 @@
         <v>25</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B98" t="s">
         <v>52</v>
@@ -3085,12 +3093,12 @@
         <v>25</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
@@ -3102,12 +3110,12 @@
         <v>25</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B100" t="s">
         <v>52</v>
@@ -3119,12 +3127,12 @@
         <v>25</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B101" t="s">
         <v>52</v>
@@ -3136,12 +3144,12 @@
         <v>25</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B102" t="s">
         <v>52</v>
@@ -3153,12 +3161,12 @@
         <v>25</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B103" t="s">
         <v>52</v>
@@ -3170,12 +3178,12 @@
         <v>25</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B104" t="s">
         <v>52</v>
@@ -3187,12 +3195,12 @@
         <v>25</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B105" t="s">
         <v>52</v>
@@ -3204,12 +3212,12 @@
         <v>25</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B106" t="s">
         <v>52</v>
@@ -3221,12 +3229,12 @@
         <v>25</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B107" t="s">
         <v>52</v>
@@ -3238,12 +3246,12 @@
         <v>25</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B108" t="s">
         <v>52</v>
@@ -3255,12 +3263,12 @@
         <v>25</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B109" t="s">
         <v>52</v>
@@ -3272,12 +3280,12 @@
         <v>25</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B110" t="s">
         <v>52</v>
@@ -3289,12 +3297,12 @@
         <v>25</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
@@ -3306,12 +3314,12 @@
         <v>25</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B112" t="s">
         <v>52</v>
@@ -3323,23 +3331,40 @@
         <v>25</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="B113" t="s">
-        <v>52</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G113" s="10" t="s">
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" s="10" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3349,78 +3374,78 @@
     <hyperlink ref="G14" r:id="rId2"/>
     <hyperlink ref="G13" r:id="rId3"/>
     <hyperlink ref="G12" r:id="rId4"/>
-    <hyperlink ref="G34" r:id="rId5"/>
-    <hyperlink ref="G35" r:id="rId6"/>
-    <hyperlink ref="G36" r:id="rId7"/>
-    <hyperlink ref="G37" r:id="rId8"/>
-    <hyperlink ref="G39" r:id="rId9"/>
-    <hyperlink ref="G40" r:id="rId10"/>
-    <hyperlink ref="G41" r:id="rId11"/>
-    <hyperlink ref="G45" r:id="rId12"/>
-    <hyperlink ref="G46" r:id="rId13"/>
-    <hyperlink ref="G47" r:id="rId14"/>
-    <hyperlink ref="G48" r:id="rId15"/>
-    <hyperlink ref="G49" r:id="rId16"/>
-    <hyperlink ref="G51" r:id="rId17"/>
-    <hyperlink ref="G55" r:id="rId18"/>
-    <hyperlink ref="G54" r:id="rId19"/>
-    <hyperlink ref="G56" r:id="rId20"/>
-    <hyperlink ref="G57" r:id="rId21"/>
-    <hyperlink ref="G58" r:id="rId22"/>
-    <hyperlink ref="G59" r:id="rId23"/>
-    <hyperlink ref="G60" r:id="rId24"/>
-    <hyperlink ref="G61" r:id="rId25"/>
-    <hyperlink ref="G62" r:id="rId26"/>
-    <hyperlink ref="G63" r:id="rId27"/>
-    <hyperlink ref="G64" r:id="rId28"/>
-    <hyperlink ref="G65" r:id="rId29"/>
-    <hyperlink ref="G66" r:id="rId30"/>
-    <hyperlink ref="G67" r:id="rId31"/>
-    <hyperlink ref="G68" r:id="rId32"/>
-    <hyperlink ref="G69" r:id="rId33"/>
-    <hyperlink ref="G53" r:id="rId34"/>
-    <hyperlink ref="G70" r:id="rId35"/>
-    <hyperlink ref="G71" r:id="rId36"/>
-    <hyperlink ref="G72" r:id="rId37"/>
-    <hyperlink ref="G73" r:id="rId38"/>
-    <hyperlink ref="G74" r:id="rId39"/>
-    <hyperlink ref="G75" r:id="rId40"/>
-    <hyperlink ref="G76" r:id="rId41"/>
-    <hyperlink ref="G77" r:id="rId42"/>
-    <hyperlink ref="G78" r:id="rId43"/>
-    <hyperlink ref="G79" r:id="rId44"/>
-    <hyperlink ref="G80" r:id="rId45"/>
-    <hyperlink ref="G82" r:id="rId46"/>
-    <hyperlink ref="G83" r:id="rId47"/>
-    <hyperlink ref="G84" r:id="rId48"/>
-    <hyperlink ref="G85" r:id="rId49"/>
-    <hyperlink ref="G86" r:id="rId50"/>
-    <hyperlink ref="G87" r:id="rId51"/>
-    <hyperlink ref="G88" r:id="rId52"/>
-    <hyperlink ref="G89" r:id="rId53"/>
-    <hyperlink ref="G90" r:id="rId54"/>
-    <hyperlink ref="G91" r:id="rId55"/>
-    <hyperlink ref="G92" r:id="rId56"/>
-    <hyperlink ref="G93" r:id="rId57"/>
-    <hyperlink ref="G94" r:id="rId58"/>
-    <hyperlink ref="G95" r:id="rId59"/>
-    <hyperlink ref="G96" r:id="rId60"/>
-    <hyperlink ref="G97" r:id="rId61"/>
-    <hyperlink ref="G98" r:id="rId62"/>
-    <hyperlink ref="G99" r:id="rId63"/>
-    <hyperlink ref="G100" r:id="rId64"/>
-    <hyperlink ref="G101" r:id="rId65"/>
-    <hyperlink ref="G102" r:id="rId66"/>
-    <hyperlink ref="G103" r:id="rId67"/>
-    <hyperlink ref="G104" r:id="rId68"/>
-    <hyperlink ref="G105" r:id="rId69"/>
-    <hyperlink ref="G106" r:id="rId70"/>
-    <hyperlink ref="G107" r:id="rId71"/>
-    <hyperlink ref="G108" r:id="rId72"/>
-    <hyperlink ref="G109" r:id="rId73"/>
-    <hyperlink ref="G110" r:id="rId74"/>
-    <hyperlink ref="G113" r:id="rId75"/>
-    <hyperlink ref="G111" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G35" r:id="rId5"/>
+    <hyperlink ref="G36" r:id="rId6"/>
+    <hyperlink ref="G37" r:id="rId7"/>
+    <hyperlink ref="G38" r:id="rId8"/>
+    <hyperlink ref="G40" r:id="rId9"/>
+    <hyperlink ref="G41" r:id="rId10"/>
+    <hyperlink ref="G42" r:id="rId11"/>
+    <hyperlink ref="G46" r:id="rId12"/>
+    <hyperlink ref="G47" r:id="rId13"/>
+    <hyperlink ref="G48" r:id="rId14"/>
+    <hyperlink ref="G49" r:id="rId15"/>
+    <hyperlink ref="G50" r:id="rId16"/>
+    <hyperlink ref="G52" r:id="rId17"/>
+    <hyperlink ref="G56" r:id="rId18"/>
+    <hyperlink ref="G55" r:id="rId19"/>
+    <hyperlink ref="G57" r:id="rId20"/>
+    <hyperlink ref="G58" r:id="rId21"/>
+    <hyperlink ref="G59" r:id="rId22"/>
+    <hyperlink ref="G60" r:id="rId23"/>
+    <hyperlink ref="G61" r:id="rId24"/>
+    <hyperlink ref="G62" r:id="rId25"/>
+    <hyperlink ref="G63" r:id="rId26"/>
+    <hyperlink ref="G64" r:id="rId27"/>
+    <hyperlink ref="G65" r:id="rId28"/>
+    <hyperlink ref="G66" r:id="rId29"/>
+    <hyperlink ref="G67" r:id="rId30"/>
+    <hyperlink ref="G68" r:id="rId31"/>
+    <hyperlink ref="G69" r:id="rId32"/>
+    <hyperlink ref="G70" r:id="rId33"/>
+    <hyperlink ref="G54" r:id="rId34"/>
+    <hyperlink ref="G71" r:id="rId35"/>
+    <hyperlink ref="G72" r:id="rId36"/>
+    <hyperlink ref="G73" r:id="rId37"/>
+    <hyperlink ref="G74" r:id="rId38"/>
+    <hyperlink ref="G75" r:id="rId39"/>
+    <hyperlink ref="G76" r:id="rId40"/>
+    <hyperlink ref="G77" r:id="rId41"/>
+    <hyperlink ref="G78" r:id="rId42"/>
+    <hyperlink ref="G79" r:id="rId43"/>
+    <hyperlink ref="G80" r:id="rId44"/>
+    <hyperlink ref="G81" r:id="rId45"/>
+    <hyperlink ref="G83" r:id="rId46"/>
+    <hyperlink ref="G84" r:id="rId47"/>
+    <hyperlink ref="G85" r:id="rId48"/>
+    <hyperlink ref="G86" r:id="rId49"/>
+    <hyperlink ref="G87" r:id="rId50"/>
+    <hyperlink ref="G88" r:id="rId51"/>
+    <hyperlink ref="G89" r:id="rId52"/>
+    <hyperlink ref="G90" r:id="rId53"/>
+    <hyperlink ref="G91" r:id="rId54"/>
+    <hyperlink ref="G92" r:id="rId55"/>
+    <hyperlink ref="G93" r:id="rId56"/>
+    <hyperlink ref="G94" r:id="rId57"/>
+    <hyperlink ref="G95" r:id="rId58"/>
+    <hyperlink ref="G96" r:id="rId59"/>
+    <hyperlink ref="G97" r:id="rId60"/>
+    <hyperlink ref="G98" r:id="rId61"/>
+    <hyperlink ref="G99" r:id="rId62"/>
+    <hyperlink ref="G100" r:id="rId63"/>
+    <hyperlink ref="G101" r:id="rId64"/>
+    <hyperlink ref="G102" r:id="rId65"/>
+    <hyperlink ref="G103" r:id="rId66"/>
+    <hyperlink ref="G104" r:id="rId67"/>
+    <hyperlink ref="G105" r:id="rId68"/>
+    <hyperlink ref="G106" r:id="rId69"/>
+    <hyperlink ref="G107" r:id="rId70"/>
+    <hyperlink ref="G108" r:id="rId71"/>
+    <hyperlink ref="G109" r:id="rId72"/>
+    <hyperlink ref="G110" r:id="rId73"/>
+    <hyperlink ref="G111" r:id="rId74"/>
+    <hyperlink ref="G114" r:id="rId75"/>
+    <hyperlink ref="G112" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>

</xml_diff>

<commit_message>
FS user was updated
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C783626
</commit_message>
<xml_diff>
--- a/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Adestra/src/test/resources/CobaltUsers.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="277">
   <si>
     <t>UserName</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Annotations user2</t>
   </si>
   <si>
-    <t>FSTestUser1</t>
-  </si>
-  <si>
     <t>FFHTestUser</t>
   </si>
   <si>
@@ -844,6 +841,12 @@
   </si>
   <si>
     <t>Password1!</t>
+  </si>
+  <si>
+    <t>FSTestUser2</t>
+  </si>
+  <si>
+    <t>Password!</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1303,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1380,7 +1383,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1401,7 +1404,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1422,7 +1425,7 @@
         <v>25</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1443,15 +1446,15 @@
         <v>25</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>61</v>
+        <v>275</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>52</v>
+        <v>276</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1483,7 +1486,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1504,7 +1507,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1525,7 +1528,7 @@
         <v>25</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1546,7 +1549,7 @@
         <v>25</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1565,7 +1568,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="3"/>
       <c r="G14" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,7 +1589,7 @@
         <v>25</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1751,10 +1754,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>6</v>
@@ -1823,10 +1826,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
@@ -1842,7 +1845,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>52</v>
@@ -1850,7 +1853,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>25</v>
@@ -1859,7 +1862,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>52</v>
@@ -1867,7 +1870,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>25</v>
@@ -1876,17 +1879,17 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>275</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>25</v>
@@ -1895,7 +1898,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>52</v>
@@ -1905,7 +1908,7 @@
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>25</v>
@@ -1914,45 +1917,45 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>52</v>
@@ -1966,12 +1969,12 @@
         <v>25</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>52</v>
@@ -1979,18 +1982,18 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>52</v>
@@ -2002,12 +2005,12 @@
         <v>25</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>52</v>
@@ -2015,37 +2018,37 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>52</v>
@@ -2057,18 +2060,18 @@
         <v>33</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>52</v>
@@ -2080,49 +2083,49 @@
         <v>33</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>25</v>
@@ -2131,19 +2134,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="E44" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>25</v>
@@ -2152,30 +2155,30 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E45" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>52</v>
@@ -2183,18 +2186,18 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>52</v>
@@ -2202,81 +2205,81 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="F48" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="F49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="F50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>52</v>
@@ -2284,18 +2287,18 @@
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>52</v>
@@ -2303,18 +2306,18 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>52</v>
@@ -2322,1050 +2325,1050 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
         <v>52</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B68" t="s">
         <v>52</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B71" t="s">
         <v>52</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B75" t="s">
         <v>52</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B76" t="s">
         <v>52</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B78" t="s">
         <v>52</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
         <v>52</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B81" t="s">
         <v>52</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B82" t="s">
         <v>52</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B83" t="s">
         <v>52</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B84" t="s">
         <v>52</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F84" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B85" t="s">
         <v>52</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F85" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B86" t="s">
         <v>52</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F86" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B87" t="s">
         <v>52</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F87" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B88" t="s">
         <v>52</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F88" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F90" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B91" t="s">
         <v>52</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F91" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B92" t="s">
         <v>52</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F92" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B93" t="s">
         <v>52</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F93" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B94" t="s">
         <v>52</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F94" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B95" t="s">
         <v>52</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F95" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B96" t="s">
         <v>52</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F96" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B97" t="s">
         <v>52</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F97" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B98" t="s">
         <v>52</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F98" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F99" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B100" t="s">
         <v>52</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F100" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B101" t="s">
         <v>52</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F101" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B102" t="s">
         <v>52</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F102" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B103" t="s">
         <v>52</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F103" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B104" t="s">
         <v>52</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F104" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B105" t="s">
         <v>52</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F105" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B106" t="s">
         <v>52</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F106" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B107" t="s">
         <v>52</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F107" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B108" t="s">
         <v>52</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F108" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B109" t="s">
         <v>52</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F109" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B110" t="s">
         <v>52</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F110" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F111" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B112" t="s">
         <v>52</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F112" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B113" t="s">
         <v>52</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F113" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G113" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B114" t="s">
         <v>52</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F114" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G114" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -3468,26 +3471,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3505,7 +3508,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>